<commit_message>
Update RS of MS-ASPROV.
</commit_message>
<xml_diff>
--- a/ExchangeActiveSync/Docs/MS-ASPROV/MS-ASPROV_RequirementSpecification.xlsx
+++ b/ExchangeActiveSync/Docs/MS-ASPROV/MS-ASPROV_RequirementSpecification.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23127"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEDC168B-5BAA-4981-8B14-3D9F5EB73AAC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A8498B7-F08D-4D87-9CE0-69192CEC6E87}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7149" uniqueCount="2170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7153" uniqueCount="2170">
   <si>
     <t>Req ID</t>
   </si>
@@ -7267,21 +7267,6 @@
     <xf numFmtId="2" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -7305,6 +7290,21 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -13333,8 +13333,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:I1031"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C820" sqref="C820"/>
+    <sheetView tabSelected="1" topLeftCell="A96" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H108" sqref="H108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -13385,120 +13385,120 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="21">
-      <c r="A4" s="45" t="s">
+      <c r="A4" s="53" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="45"/>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45"/>
+      <c r="B4" s="53"/>
+      <c r="C4" s="53"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="53"/>
+      <c r="F4" s="53"/>
+      <c r="G4" s="53"/>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="48" t="s">
+      <c r="B5" s="56" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="49"/>
-      <c r="D5" s="49"/>
-      <c r="E5" s="49"/>
-      <c r="F5" s="49"/>
-      <c r="G5" s="49"/>
-      <c r="H5" s="49"/>
-      <c r="I5" s="49"/>
+      <c r="C5" s="57"/>
+      <c r="D5" s="57"/>
+      <c r="E5" s="57"/>
+      <c r="F5" s="57"/>
+      <c r="G5" s="57"/>
+      <c r="H5" s="57"/>
+      <c r="I5" s="57"/>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="47" t="s">
+      <c r="B6" s="55" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="47"/>
-      <c r="D6" s="47"/>
-      <c r="E6" s="47"/>
-      <c r="F6" s="47"/>
-      <c r="G6" s="47"/>
-      <c r="H6" s="47"/>
-      <c r="I6" s="47"/>
+      <c r="C6" s="55"/>
+      <c r="D6" s="55"/>
+      <c r="E6" s="55"/>
+      <c r="F6" s="55"/>
+      <c r="G6" s="55"/>
+      <c r="H6" s="55"/>
+      <c r="I6" s="55"/>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="B7" s="46" t="s">
+      <c r="B7" s="54" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="46"/>
-      <c r="D7" s="46"/>
-      <c r="E7" s="46"/>
-      <c r="F7" s="46"/>
-      <c r="G7" s="46"/>
-      <c r="H7" s="46"/>
-      <c r="I7" s="46"/>
+      <c r="C7" s="54"/>
+      <c r="D7" s="54"/>
+      <c r="E7" s="54"/>
+      <c r="F7" s="54"/>
+      <c r="G7" s="54"/>
+      <c r="H7" s="54"/>
+      <c r="I7" s="54"/>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="46" t="s">
+      <c r="B8" s="54" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="46"/>
-      <c r="D8" s="46"/>
-      <c r="E8" s="46"/>
-      <c r="F8" s="46"/>
-      <c r="G8" s="46"/>
-      <c r="H8" s="46"/>
-      <c r="I8" s="46"/>
+      <c r="C8" s="54"/>
+      <c r="D8" s="54"/>
+      <c r="E8" s="54"/>
+      <c r="F8" s="54"/>
+      <c r="G8" s="54"/>
+      <c r="H8" s="54"/>
+      <c r="I8" s="54"/>
     </row>
     <row r="9" spans="1:9" ht="78.75" customHeight="1">
       <c r="A9" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="54" t="s">
+      <c r="B9" s="49" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="55"/>
-      <c r="D9" s="55"/>
-      <c r="E9" s="55"/>
-      <c r="F9" s="55"/>
-      <c r="G9" s="55"/>
-      <c r="H9" s="55"/>
-      <c r="I9" s="55"/>
+      <c r="C9" s="50"/>
+      <c r="D9" s="50"/>
+      <c r="E9" s="50"/>
+      <c r="F9" s="50"/>
+      <c r="G9" s="50"/>
+      <c r="H9" s="50"/>
+      <c r="I9" s="50"/>
     </row>
     <row r="10" spans="1:9" ht="33.75" customHeight="1">
       <c r="A10" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="54" t="s">
+      <c r="B10" s="49" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="55"/>
-      <c r="D10" s="55"/>
-      <c r="E10" s="55"/>
-      <c r="F10" s="55"/>
-      <c r="G10" s="55"/>
-      <c r="H10" s="55"/>
-      <c r="I10" s="55"/>
+      <c r="C10" s="50"/>
+      <c r="D10" s="50"/>
+      <c r="E10" s="50"/>
+      <c r="F10" s="50"/>
+      <c r="G10" s="50"/>
+      <c r="H10" s="50"/>
+      <c r="I10" s="50"/>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="50" t="s">
+      <c r="B11" s="45" t="s">
         <v>37</v>
       </c>
-      <c r="C11" s="50"/>
-      <c r="D11" s="50"/>
-      <c r="E11" s="50"/>
-      <c r="F11" s="50"/>
-      <c r="G11" s="50"/>
-      <c r="H11" s="50"/>
-      <c r="I11" s="50"/>
+      <c r="C11" s="45"/>
+      <c r="D11" s="45"/>
+      <c r="E11" s="45"/>
+      <c r="F11" s="45"/>
+      <c r="G11" s="45"/>
+      <c r="H11" s="45"/>
+      <c r="I11" s="45"/>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="24" t="s">
@@ -13510,12 +13510,12 @@
       <c r="C12" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="51"/>
-      <c r="E12" s="51"/>
-      <c r="F12" s="51"/>
-      <c r="G12" s="51"/>
-      <c r="H12" s="51"/>
-      <c r="I12" s="51"/>
+      <c r="D12" s="46"/>
+      <c r="E12" s="46"/>
+      <c r="F12" s="46"/>
+      <c r="G12" s="46"/>
+      <c r="H12" s="46"/>
+      <c r="I12" s="46"/>
     </row>
     <row r="13" spans="1:9" ht="15" customHeight="1">
       <c r="A13" s="25" t="s">
@@ -13527,12 +13527,12 @@
       <c r="C13" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="52"/>
-      <c r="E13" s="52"/>
-      <c r="F13" s="52"/>
-      <c r="G13" s="52"/>
-      <c r="H13" s="52"/>
-      <c r="I13" s="52"/>
+      <c r="D13" s="47"/>
+      <c r="E13" s="47"/>
+      <c r="F13" s="47"/>
+      <c r="G13" s="47"/>
+      <c r="H13" s="47"/>
+      <c r="I13" s="47"/>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="25" t="s">
@@ -13544,12 +13544,12 @@
       <c r="C14" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="D14" s="52"/>
-      <c r="E14" s="52"/>
-      <c r="F14" s="52"/>
-      <c r="G14" s="52"/>
-      <c r="H14" s="52"/>
-      <c r="I14" s="52"/>
+      <c r="D14" s="47"/>
+      <c r="E14" s="47"/>
+      <c r="F14" s="47"/>
+      <c r="G14" s="47"/>
+      <c r="H14" s="47"/>
+      <c r="I14" s="47"/>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="26" t="s">
@@ -13561,57 +13561,57 @@
       <c r="C15" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="53"/>
-      <c r="E15" s="53"/>
-      <c r="F15" s="53"/>
-      <c r="G15" s="53"/>
-      <c r="H15" s="53"/>
-      <c r="I15" s="53"/>
+      <c r="D15" s="48"/>
+      <c r="E15" s="48"/>
+      <c r="F15" s="48"/>
+      <c r="G15" s="48"/>
+      <c r="H15" s="48"/>
+      <c r="I15" s="48"/>
     </row>
     <row r="16" spans="1:9" ht="30" customHeight="1">
       <c r="A16" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="50" t="s">
+      <c r="B16" s="45" t="s">
         <v>38</v>
       </c>
-      <c r="C16" s="50"/>
-      <c r="D16" s="50"/>
-      <c r="E16" s="50"/>
-      <c r="F16" s="50"/>
-      <c r="G16" s="50"/>
-      <c r="H16" s="50"/>
-      <c r="I16" s="50"/>
+      <c r="C16" s="45"/>
+      <c r="D16" s="45"/>
+      <c r="E16" s="45"/>
+      <c r="F16" s="45"/>
+      <c r="G16" s="45"/>
+      <c r="H16" s="45"/>
+      <c r="I16" s="45"/>
     </row>
     <row r="17" spans="1:9" ht="64.5" customHeight="1">
       <c r="A17" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="56" t="s">
+      <c r="B17" s="51" t="s">
         <v>39</v>
       </c>
-      <c r="C17" s="57"/>
-      <c r="D17" s="57"/>
-      <c r="E17" s="57"/>
-      <c r="F17" s="57"/>
-      <c r="G17" s="57"/>
-      <c r="H17" s="57"/>
-      <c r="I17" s="57"/>
+      <c r="C17" s="52"/>
+      <c r="D17" s="52"/>
+      <c r="E17" s="52"/>
+      <c r="F17" s="52"/>
+      <c r="G17" s="52"/>
+      <c r="H17" s="52"/>
+      <c r="I17" s="52"/>
     </row>
     <row r="18" spans="1:9" ht="30" customHeight="1">
       <c r="A18" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="50" t="s">
+      <c r="B18" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="C18" s="50"/>
-      <c r="D18" s="50"/>
-      <c r="E18" s="50"/>
-      <c r="F18" s="50"/>
-      <c r="G18" s="50"/>
-      <c r="H18" s="50"/>
-      <c r="I18" s="50"/>
+      <c r="C18" s="45"/>
+      <c r="D18" s="45"/>
+      <c r="E18" s="45"/>
+      <c r="F18" s="45"/>
+      <c r="G18" s="45"/>
+      <c r="H18" s="45"/>
+      <c r="I18" s="45"/>
     </row>
     <row r="19" spans="1:9" s="42" customFormat="1" ht="28.8">
       <c r="A19" s="3" t="s">
@@ -15793,6 +15793,18 @@
       <c r="C106" s="19" t="s">
         <v>1824</v>
       </c>
+      <c r="E106" s="41" t="s">
+        <v>19</v>
+      </c>
+      <c r="F106" s="41" t="s">
+        <v>3</v>
+      </c>
+      <c r="G106" s="41" t="s">
+        <v>15</v>
+      </c>
+      <c r="H106" s="41" t="s">
+        <v>18</v>
+      </c>
       <c r="I106" s="44"/>
     </row>
     <row r="107" spans="1:9" s="41" customFormat="1" ht="28.8">
@@ -38900,6 +38912,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B5:I5"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="D12:I15"/>
     <mergeCell ref="B16:I16"/>
@@ -38907,11 +38924,6 @@
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B17:I17"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B5:I5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A284:I284 D963:E963 A876:E876 A1018:I1029 A296:I296 I102:I106 A118:I118 I113:I117 A130:I130 I125:I129 A141:I141 I136:I140 A153:I153 I148:I152 A164:I164 I159:I163 A176:I176 I171:I175 A188:I188 I183:I187 A199:I199 I194:I198 A211:I211 I206:I210 A225:I225 I220:I224 A237:I237 I232:I236 A248:I248 I243:I247 A260:I260 I255:I259 A272:I272 I267:I271 A308:I308 I303:I307 A321:I321 I316:I320 A331:I331 I326:I330 A344:I344 I339:I343 I350:I354 A365:I365 I360:I364 A376:I376 I371:I375 A390:I390 I385:I389 I399:I403 A413:I413 I408:I412 A423:I423 I418:I422 A433:I433 I428:I432 A447:I447 I442:I446 A459:I459 I454:I458 A474:I474 I469:I473 A486:I486 I481:I485 A498:I498 I493:I497 I503:I507 A520:I520 I515:I519 I526:I530 A549:I549 I544:I548 I552:I556 A569:I569 I564:I568 A580:I580 I575:I579 A591:I591 I585:I589 A598:I598 I593:I597 A608:I608 I603:I607 A619:I619 I614:I618 A630:I630 I625:I629 A644:I644 I639:I643 A655:I655 I650:I654 A666:I666 I661:I665 A677:I677 I672:I676 I684:I688 A727:I727 I722:I726 A740:I740 I735:I739 A751:I751 I746:I750 I758:I762 A355:I355 C590:I590 A956:C956 E956:I956 A877:I892 A957:I962 C107:I112 C95:I101 B95:B106 A20:I94 C119:I124 A119:A129 C131:I135 A131:A140 C142:I147 A142:A152 A154:A163 C154:I158 A165:A175 C165:I170 A177:A187 C177:I182 A189:A198 C189:I193 C200:I205 A200:A210 C212:I219 A212:A224 C226:I231 A226:A236 C238:I242 A238:A247 C249:I254 A249:A259 C261:I266 A261:A271 C273:I277 C278:E278 A273:A283 C290:E290 C285:I289 A285:A295 C297:I302 A297:A307 C309:I315 A309:A320 C322:I325 A322:A330 C332:I338 A332:A343 A345:A353 C345:I349 A354:B354 C356:I359 A356:A364 C366:I370 A366:A375 C377:I384 A377:A389 C391:I398 A391:A403 A404:I407 A408:B412 C414:I417 A414:A422 C424:I427 A424:A432 C434:I441 A434:A446 C448:I453 A448:A458 C460:I468 A460:A473 C475:I480 A475:A485 C487:I492 A487:A497 C499:I502 A499:A507 A508:I514 A515:B519 C521:I525 A521:A530 A531:I541 C542:I543 A542:A548 C550:I551 A550:A556 A557:I562 C563:I563 A563:A568 C570:I574 A570:A579 C581:I584 A581:A590 C592:I592 A592:A597 C599:I602 A599:A607 C609:I613 A609:A618 C620:I624 A620:A629 C631:I638 A631:A643 C645:I649 A645:A654 C656:I660 A656:A665 C667:I671 A667:A676 C678:I683 A678:A688 A689:I717 C718:I721 A718:A726 C728:I734 A728:A739 C741:I745 A741:A750 C752:I757 A752:A762 A763:I828 A829:A833 C829:I833 A834:I875 A894:I955 A964:B1017 D964:I1017 A95:A117">
@@ -42671,15 +42683,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F2EA47BB262D974097182E2CA8AB13E1" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="74597e8d9e42e7e4fc8eda6d37675aa2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4aeb20c0e3442673af7ee10786458764">
     <xsd:element name="properties">
@@ -42728,6 +42731,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
   <documentManagement/>
@@ -42735,14 +42747,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDB2DE12-5EF6-4CF2-820D-5F9FE329E08E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -42753,6 +42757,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>